<commit_message>
Autocorrelation has been fixed
</commit_message>
<xml_diff>
--- a/data_lab1.xlsx
+++ b/data_lab1.xlsx
@@ -338,10 +338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H300"/>
+  <dimension ref="A1:A300"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -350,90 +350,82 @@
     <col min="5" max="5" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>107.28158389327129</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>127.82735370530034</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>408.3546686385011</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>98.890546210211852</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>701.75957763374743</v>
       </c>
-      <c r="H5">
-        <f>VAR(A1:A300)</f>
-        <v>29298.173050900965</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>271.81439391360277</v>
       </c>
-      <c r="H6">
-        <f>_xlfn.STDEV.S(A1:A300)</f>
-        <v>171.16709102774681</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>320.49549343299248</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>248.02335172534512</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>224.91195357298182</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>454.21521094440101</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>254.47077882330547</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>216.90657928262164</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>797.62537343667645</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>630.35309829085122</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>187.66933410519863</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>81.610533594883279</v>
       </c>

</xml_diff>

<commit_message>
added calc correlation function
</commit_message>
<xml_diff>
--- a/data_lab1.xlsx
+++ b/data_lab1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\PycharmProjects\Modelling_Lab1\"/>
@@ -12,14 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8790"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -31,7 +26,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -55,15 +49,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -76,9 +69,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -86,44 +79,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -150,15 +143,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -185,10 +177,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -197,142 +188,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -340,1518 +355,1513 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A275" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>107.28158389327129</v>
+      <c r="A1">
+        <v>107.2815838932713</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>127.82735370530034</v>
+      <c r="A2">
+        <v>127.8273537053003</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>408.3546686385011</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>98.890546210211852</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>701.75957763374743</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>271.81439391360277</v>
+      <c r="A6">
+        <v>271.81439391360283</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>320.49549343299248</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>248.02335172534512</v>
+      <c r="A8">
+        <v>248.02335172534509</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>224.91195357298182</v>
+      <c r="A9">
+        <v>224.91195357298179</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>454.21521094440101</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>254.47077882330547</v>
+      <c r="A11">
+        <v>254.47077882330549</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>216.90657928262164</v>
+      <c r="A12">
+        <v>216.90657928262161</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>797.62537343667645</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>630.35309829085122</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>187.66933410519863</v>
+      <c r="A15">
+        <v>187.6693341051986</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>81.610533594883279</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>283.24936593557317</v>
+      <c r="A17">
+        <v>283.24936593557322</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>151.51033225013779</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>407.89408014857736</v>
+      <c r="A19">
+        <v>407.89408014857742</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>196.50012539926712</v>
+      <c r="A20">
+        <v>196.50012539926709</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>226.10190058519862</v>
+      <c r="A21">
+        <v>226.10190058519859</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>296.82006676145301</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>365.89967866417624</v>
+      <c r="A23">
+        <v>365.89967866417618</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>126.08793960916096</v>
+      <c r="A24">
+        <v>126.087939609161</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25">
         <v>158.17331398046889</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26">
         <v>169.31814511084991</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>356.99176152030975</v>
+      <c r="A27">
+        <v>356.99176152030981</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28">
         <v>51.531820594945302</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>138.94007100937398</v>
+      <c r="A29">
+        <v>138.94007100937401</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>122.36436339055496</v>
+      <c r="A30">
+        <v>122.364363390555</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>192.42385978046303</v>
+      <c r="A31">
+        <v>192.423859780463</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>314.19161734563977</v>
+      <c r="A32">
+        <v>314.19161734563983</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>224.76623940791234</v>
+      <c r="A33">
+        <v>224.76623940791231</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34">
         <v>55.898927187361181</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>327.76712307497064</v>
+      <c r="A35">
+        <v>327.76712307497058</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36">
         <v>375.33573039261597</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>227.86161586375553</v>
+      <c r="A37">
+        <v>227.8616158637555</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+      <c r="A38">
         <v>355.13663052220119</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="A39">
         <v>286.7413177403497</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>133.99561157809518</v>
+      <c r="A40">
+        <v>133.99561157809521</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>229.31356051547908</v>
+      <c r="A41">
+        <v>229.31356051547911</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="A42">
         <v>427.5796519704889</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>379.88380148467013</v>
+      <c r="A43">
+        <v>379.88380148467007</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>470.07277475710123</v>
+      <c r="A44">
+        <v>470.07277475710117</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>270.68980051071156</v>
+      <c r="A45">
+        <v>270.68980051071162</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>151.08022269670758</v>
+      <c r="A46">
+        <v>151.08022269670761</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>184.74179118427588</v>
+      <c r="A47">
+        <v>184.74179118427591</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+      <c r="A48">
         <v>484.80314732117779</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="A49">
         <v>130.8094017575973</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>184.10637657715995</v>
+      <c r="A50">
+        <v>184.10637657715989</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+      <c r="A51">
         <v>385.10511983287188</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
+      <c r="A52">
         <v>83.235214760513699</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>195.65674454690125</v>
+      <c r="A53">
+        <v>195.65674454690131</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
+      <c r="A54">
         <v>540.52449203860169</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>343.16788171818587</v>
+      <c r="A55">
+        <v>343.16788171818592</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+      <c r="A56">
         <v>377.46792019065362</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+      <c r="A57">
         <v>763.05828906878878</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+      <c r="A58">
         <v>114.1957280012459</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+      <c r="A59">
         <v>93.828691587588537</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+      <c r="A60">
         <v>288.55840885143232</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+      <c r="A61">
         <v>527.20635732889855</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+      <c r="A62">
         <v>684.17142200543822</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>318.45739323918156</v>
+      <c r="A63">
+        <v>318.45739323918161</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+      <c r="A64">
         <v>208.72149310978941</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>246.93208789280652</v>
+      <c r="A65">
+        <v>246.93208789280649</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
-        <v>135.05870598078235</v>
+      <c r="A66">
+        <v>135.05870598078229</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <v>212.00109132019526</v>
+      <c r="A67">
+        <v>212.00109132019529</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+      <c r="A68">
         <v>65.071926371309047</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>477.48731714154536</v>
+      <c r="A69">
+        <v>477.48731714154542</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+      <c r="A70">
         <v>379.10072832547741</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+      <c r="A71">
         <v>419.18061229105331</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
+      <c r="A72">
         <v>92.051072390415982</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>505.15934999217063</v>
+      <c r="A73">
+        <v>505.15934999217058</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>204.64797660269062</v>
+      <c r="A74">
+        <v>204.64797660269059</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+      <c r="A75">
         <v>393.69557760716901</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
+      <c r="A76">
         <v>208.3377473171555</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <v>131.10075713382952</v>
+      <c r="A77">
+        <v>131.10075713382949</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>200.34605210648334</v>
+      <c r="A78">
+        <v>200.34605210648331</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>220.18785541026077</v>
+      <c r="A79">
+        <v>220.18785541026079</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
+      <c r="A80">
         <v>545.34426792191391</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <v>298.21504684333127</v>
+      <c r="A81">
+        <v>298.21504684333132</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <v>35.333966596066375</v>
+      <c r="A82">
+        <v>35.333966596066382</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
-        <v>185.44794327967338</v>
+      <c r="A83">
+        <v>185.44794327967341</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
+      <c r="A84">
         <v>436.56347628770209</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
-        <v>162.67977861718344</v>
+      <c r="A85">
+        <v>162.67977861718339</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <v>216.15215722346178</v>
+      <c r="A86">
+        <v>216.15215722346181</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
-        <v>249.61201762606564</v>
+      <c r="A87">
+        <v>249.61201762606561</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
-        <v>341.69175316393586</v>
+      <c r="A88">
+        <v>341.69175316393591</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <v>203.30563183272307</v>
+      <c r="A89">
+        <v>203.30563183272309</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
-        <v>388.73073722723774</v>
+      <c r="A90">
+        <v>388.73073722723768</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
-        <v>158.91079043238744</v>
+      <c r="A91">
+        <v>158.91079043238739</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+      <c r="A92">
         <v>79.627903538835881</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
-        <v>127.99124370748665</v>
+      <c r="A93">
+        <v>127.9912437074866</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+      <c r="A94">
         <v>395.60937797206873</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
-        <v>211.19042812250598</v>
+      <c r="A95">
+        <v>211.19042812250601</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+      <c r="A96">
         <v>336.1261218728319</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+      <c r="A97">
         <v>283.75273249906081</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
-        <v>105.02116918454753</v>
+      <c r="A98">
+        <v>105.0211691845475</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
-        <v>425.36850075864334</v>
+      <c r="A99">
+        <v>425.36850075864328</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <v>102.97001833383734</v>
+      <c r="A100">
+        <v>102.9700183338373</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
-        <v>366.03119660905475</v>
+      <c r="A101">
+        <v>366.03119660905469</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
-        <v>340.31592031699176</v>
+      <c r="A102">
+        <v>340.31592031699182</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
+      <c r="A103">
         <v>89.406776230258188</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
+      <c r="A104">
         <v>86.036017111450917</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
+      <c r="A105">
         <v>180.52809446994971</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
-        <v>156.25047183375975</v>
+      <c r="A106">
+        <v>156.25047183375969</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
+      <c r="A107">
         <v>348.9796212775168</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
+      <c r="A108">
         <v>26.25929918955304</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
+      <c r="A109">
         <v>203.68345331447091</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
-        <v>102.17919882822795</v>
+      <c r="A110">
+        <v>102.179198828228</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
-        <v>190.51609288178926</v>
+      <c r="A111">
+        <v>190.51609288178929</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
-        <v>235.64677760754643</v>
+      <c r="A112">
+        <v>235.6467776075464</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
-        <v>250.73257522774867</v>
+      <c r="A113">
+        <v>250.7325752277487</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
+      <c r="A114">
         <v>124.48179450312151</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
+      <c r="A115">
         <v>87.931068082034301</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
-        <v>321.42360626576317</v>
+      <c r="A116">
+        <v>321.42360626576323</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
-        <v>190.79671678950294</v>
+      <c r="A117">
+        <v>190.79671678950291</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
+      <c r="A118">
         <v>86.592257298542492</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
+      <c r="A119">
         <v>474.05599626791059</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
-        <v>108.43545068003378</v>
+      <c r="A120">
+        <v>108.4354506800338</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
+      <c r="A121">
         <v>442.97592651122511</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
-        <v>314.68068213842207</v>
+      <c r="A122">
+        <v>314.68068213842213</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
+      <c r="A123">
         <v>536.39248842962934</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
-        <v>220.93049742013136</v>
+      <c r="A124">
+        <v>220.93049742013139</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
-        <v>255.22691671136863</v>
+      <c r="A125">
+        <v>255.2269167113686</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
+      <c r="A126">
         <v>135.59061651296579</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
+      <c r="A127">
         <v>472.47974649011212</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="1">
+      <c r="A128">
         <v>679.95273325503615</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
-        <v>117.46470521298471</v>
+      <c r="A129">
+        <v>117.4647052129847</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
+      <c r="A130">
         <v>59.92031507532073</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="1">
+      <c r="A131">
         <v>187.10412979569011</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="1">
-        <v>251.00913706758195</v>
+      <c r="A132">
+        <v>251.00913706758189</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="1">
+      <c r="A133">
         <v>218.43906919934599</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="1">
-        <v>434.82516443016164</v>
+      <c r="A134">
+        <v>434.82516443016158</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="1">
-        <v>221.11042209559358</v>
+      <c r="A135">
+        <v>221.11042209559361</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="1">
-        <v>172.53484271505926</v>
+      <c r="A136">
+        <v>172.53484271505931</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="1">
+      <c r="A137">
         <v>495.71101325955192</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="1">
+      <c r="A138">
         <v>213.86728633348781</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="1">
+      <c r="A139">
         <v>511.496427037648</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="1">
+      <c r="A140">
         <v>74.011159316182813</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="1">
-        <v>206.16605378324252</v>
+      <c r="A141">
+        <v>206.16605378324249</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="1">
+      <c r="A142">
         <v>76.461815482975467</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
+      <c r="A143">
         <v>47.67542915595395</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
-        <v>291.17677702452175</v>
+      <c r="A144">
+        <v>291.17677702452181</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
+      <c r="A145">
         <v>134.87230332402521</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
+      <c r="A146">
         <v>199.11543644843971</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
+      <c r="A147">
         <v>530.99578288292787</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="1">
-        <v>20.670413649223192</v>
+      <c r="A148">
+        <v>20.670413649223189</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="1">
-        <v>284.26678006048337</v>
+      <c r="A149">
+        <v>284.26678006048343</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="1">
+      <c r="A150">
         <v>82.119068833463558</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="1">
+      <c r="A151">
         <v>376.28476153968569</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="1">
+      <c r="A152">
         <v>89.209363168845584</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="1">
-        <v>422.97353373003557</v>
+      <c r="A153">
+        <v>422.97353373003563</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="1">
-        <v>186.37499794933927</v>
+      <c r="A154">
+        <v>186.3749979493393</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
+      <c r="A155">
         <v>275.58962231740099</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="1">
-        <v>279.71092227464675</v>
+      <c r="A156">
+        <v>279.71092227464669</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="1">
+      <c r="A157">
         <v>256.5777260229512</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="1">
-        <v>339.84848550874926</v>
+      <c r="A158">
+        <v>339.84848550874932</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="1">
+      <c r="A159">
         <v>91.16298936540359</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="1">
-        <v>371.57228795950266</v>
+      <c r="A160">
+        <v>371.57228795950272</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="1">
+      <c r="A161">
         <v>165.73533880031849</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="1">
-        <v>431.84785533197737</v>
+      <c r="A162">
+        <v>431.84785533197743</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="1">
+      <c r="A163">
         <v>518.50225693162645</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="1">
+      <c r="A164">
         <v>597.67486927964592</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="1">
+      <c r="A165">
         <v>70.562148340304248</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="1">
+      <c r="A166">
         <v>161.71169634723401</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="1">
-        <v>365.92766702071486</v>
+      <c r="A167">
+        <v>365.92766702071492</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="1">
+      <c r="A168">
         <v>377.45761753511613</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="1">
-        <v>244.57049680440883</v>
+      <c r="A169">
+        <v>244.5704968044088</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="1">
-        <v>380.53299535209015</v>
+      <c r="A170">
+        <v>380.53299535209021</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="1">
+      <c r="A171">
         <v>119.77504990150319</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="1">
-        <v>218.24048797629771</v>
+      <c r="A172">
+        <v>218.24048797629769</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="1">
+      <c r="A173">
         <v>354.80386610839338</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="1">
-        <v>200.41425382552194</v>
+      <c r="A174">
+        <v>200.41425382552191</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="1">
+      <c r="A175">
         <v>214.707941943381</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="1">
-        <v>128.24713187599914</v>
+      <c r="A176">
+        <v>128.24713187599909</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="1">
-        <v>205.95740635096305</v>
+      <c r="A177">
+        <v>205.95740635096311</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="1">
-        <v>321.52646634498285</v>
+      <c r="A178">
+        <v>321.52646634498291</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="1">
-        <v>288.73933496950207</v>
+      <c r="A179">
+        <v>288.73933496950212</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="1">
-        <v>235.36159506521165</v>
+      <c r="A180">
+        <v>235.36159506521159</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="1">
+      <c r="A181">
         <v>536.03507312259637</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="1">
+      <c r="A182">
         <v>228.25600047470829</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="1">
-        <v>215.51690149816432</v>
+      <c r="A183">
+        <v>215.51690149816429</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" s="1">
+      <c r="A184">
         <v>172.97098123856031</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="1">
-        <v>298.65735848541505</v>
+      <c r="A185">
+        <v>298.65735848541499</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="1">
-        <v>157.53435581019252</v>
+      <c r="A186">
+        <v>157.53435581019249</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="1">
+      <c r="A187">
         <v>84.03211744007605</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="1">
+      <c r="A188">
         <v>188.71752493582289</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="1">
-        <v>116.60437593747307</v>
+      <c r="A189">
+        <v>116.60437593747309</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="1">
-        <v>134.94640883037687</v>
+      <c r="A190">
+        <v>134.9464088303769</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" s="1">
+      <c r="A191">
         <v>435.11415526329688</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="1">
+      <c r="A192">
         <v>177.72815000706601</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="1">
-        <v>134.98922638929375</v>
+      <c r="A193">
+        <v>134.98922638929369</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="1">
+      <c r="A194">
         <v>726.69771335095948</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="1">
-        <v>37.717606599446796</v>
+      <c r="A195">
+        <v>37.717606599446803</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="1">
+      <c r="A196">
         <v>110.9162647661596</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="1">
+      <c r="A197">
         <v>416.9380434712856</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="1">
+      <c r="A198">
         <v>463.39474499202589</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="1">
+      <c r="A199">
         <v>445.64779833094963</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="1">
+      <c r="A200">
         <v>90.023263673380285</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" s="1">
-        <v>111.84495600627909</v>
+      <c r="A201">
+        <v>111.84495600627911</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="1">
-        <v>162.30978025416906</v>
+      <c r="A202">
+        <v>162.30978025416911</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="1">
-        <v>234.84640082560213</v>
+      <c r="A203">
+        <v>234.8464008256021</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="1">
+      <c r="A204">
         <v>66.950234133569865</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="1">
+      <c r="A205">
         <v>177.5374219583199</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="1">
-        <v>239.54245962962358</v>
+      <c r="A206">
+        <v>239.54245962962361</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" s="1">
+      <c r="A207">
         <v>291.72591184571502</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="1">
-        <v>186.39378572164745</v>
+      <c r="A208">
+        <v>186.39378572164739</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="1">
-        <v>392.71613683829855</v>
+      <c r="A209">
+        <v>392.71613683829861</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="1">
-        <v>310.43986982567407</v>
+      <c r="A210">
+        <v>310.43986982567412</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="1">
+      <c r="A211">
         <v>79.840544827341972</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" s="1">
-        <v>119.33915218619305</v>
+      <c r="A212">
+        <v>119.339152186193</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="1">
-        <v>367.23302635699696</v>
+      <c r="A213">
+        <v>367.23302635699702</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="1">
-        <v>486.35828173205414</v>
+      <c r="A214">
+        <v>486.35828173205408</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" s="1">
+      <c r="A215">
         <v>256.05518500026949</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="1">
+      <c r="A216">
         <v>285.08298599277799</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" s="1">
-        <v>241.71401619990274</v>
+      <c r="A217">
+        <v>241.71401619990269</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" s="1">
-        <v>193.87040170218972</v>
+      <c r="A218">
+        <v>193.8704017021897</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="1">
+      <c r="A219">
         <v>523.79082837137696</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" s="1">
+      <c r="A220">
         <v>315.01964194717908</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A221" s="1">
+      <c r="A221">
         <v>865.33275330337858</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" s="1">
+      <c r="A222">
         <v>194.59370822675589</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" s="1">
-        <v>387.39636318795874</v>
+      <c r="A223">
+        <v>387.39636318795868</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" s="1">
+      <c r="A224">
         <v>271.6269917213491</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" s="1">
+      <c r="A225">
         <v>480.38449609376869</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" s="1">
+      <c r="A226">
         <v>451.21034960551799</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" s="1">
-        <v>332.09111879125544</v>
+      <c r="A227">
+        <v>332.09111879125538</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228" s="1">
+      <c r="A228">
         <v>512.84909718625829</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" s="1">
-        <v>122.96997606972863</v>
+      <c r="A229">
+        <v>122.9699760697286</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" s="1">
+      <c r="A230">
         <v>480.00664323151329</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A231" s="1">
+      <c r="A231">
         <v>330.10248607640631</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" s="1">
+      <c r="A232">
         <v>459.81737145887951</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" s="1">
-        <v>184.61188525349203</v>
+      <c r="A233">
+        <v>184.61188525349201</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" s="1">
-        <v>346.98833471843756</v>
+      <c r="A234">
+        <v>346.98833471843761</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" s="1">
-        <v>460.73292823690343</v>
+      <c r="A235">
+        <v>460.73292823690338</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" s="1">
+      <c r="A236">
         <v>467.9847413320195</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A237" s="1">
+      <c r="A237">
         <v>77.622403875490676</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" s="1">
-        <v>119.58825745841665</v>
+      <c r="A238">
+        <v>119.58825745841661</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" s="1">
-        <v>309.06163789052243</v>
+      <c r="A239">
+        <v>309.06163789052238</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A240" s="1">
-        <v>184.82720896225106</v>
+      <c r="A240">
+        <v>184.82720896225109</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" s="1">
-        <v>371.43707688508533</v>
+      <c r="A241">
+        <v>371.43707688508528</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A242" s="1">
-        <v>200.06010326821254</v>
+      <c r="A242">
+        <v>200.06010326821249</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" s="1">
-        <v>208.77621431110893</v>
+      <c r="A243">
+        <v>208.7762143111089</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" s="1">
-        <v>292.37011409145134</v>
+      <c r="A244">
+        <v>292.37011409145128</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="1">
+      <c r="A245">
         <v>264.26874188234132</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" s="1">
+      <c r="A246">
         <v>429.0765170360126</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" s="1">
+      <c r="A247">
         <v>867.77584494766484</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" s="1">
-        <v>130.81690961984725</v>
+      <c r="A248">
+        <v>130.81690961984731</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A249" s="1">
-        <v>184.54945804544684</v>
+      <c r="A249">
+        <v>184.54945804544681</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" s="1">
-        <v>142.39879947909134</v>
+      <c r="A250">
+        <v>142.39879947909131</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" s="1">
-        <v>291.26399274604813</v>
+      <c r="A251">
+        <v>291.26399274604807</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" s="1">
-        <v>179.83761527092958</v>
+      <c r="A252">
+        <v>179.8376152709296</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" s="1">
+      <c r="A253">
         <v>79.013566197284092</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" s="1">
+      <c r="A254">
         <v>424.13906377686402</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" s="1">
-        <v>210.27814426747537</v>
+      <c r="A255">
+        <v>210.2781442674754</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" s="1">
+      <c r="A256">
         <v>334.75080264001713</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" s="1">
+      <c r="A257">
         <v>518.77563511668131</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" s="1">
-        <v>61.397898222383425</v>
+      <c r="A258">
+        <v>61.397898222383432</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A259" s="1">
+      <c r="A259">
         <v>281.6184921872071</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" s="1">
+      <c r="A260">
         <v>290.77485568812358</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" s="1">
+      <c r="A261">
         <v>620.76555402821157</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" s="1">
+      <c r="A262">
         <v>277.16883007229029</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" s="1">
-        <v>130.53417702164145</v>
+      <c r="A263">
+        <v>130.53417702164151</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" s="1">
+      <c r="A264">
         <v>224.6911762536235</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A265" s="1">
+      <c r="A265">
         <v>91.293203068559166</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" s="1">
-        <v>489.83729786120944</v>
+      <c r="A266">
+        <v>489.83729786120938</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267" s="1">
-        <v>171.93808248286928</v>
+      <c r="A267">
+        <v>171.93808248286931</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" s="1">
-        <v>127.74069801309761</v>
+      <c r="A268">
+        <v>127.7406980130976</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" s="1">
+      <c r="A269">
         <v>662.8111931353335</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" s="1">
+      <c r="A270">
         <v>313.04575332232662</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" s="1">
+      <c r="A271">
         <v>310.21369813644799</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" s="1">
+      <c r="A272">
         <v>92.858391169629328</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A273" s="1">
-        <v>124.30171322792503</v>
+      <c r="A273">
+        <v>124.30171322792501</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" s="1">
+      <c r="A274">
         <v>323.14036860304128</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" s="1">
-        <v>149.17970318256215</v>
+      <c r="A275">
+        <v>149.17970318256221</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" s="1">
+      <c r="A276">
         <v>80.646400483547254</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" s="1">
+      <c r="A277">
         <v>454.99203276299579</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" s="1">
+      <c r="A278">
         <v>332.40057234751691</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A279" s="1">
+      <c r="A279">
         <v>612.4557931085468</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" s="1">
+      <c r="A280">
         <v>572.58474270260967</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" s="1">
+      <c r="A281">
         <v>56.083659595874558</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282" s="1">
+      <c r="A282">
         <v>329.4403542661974</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" s="1">
+      <c r="A283">
         <v>365.64599340118349</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" s="1">
-        <v>126.82603233645506</v>
+      <c r="A284">
+        <v>126.8260323364551</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" s="1">
-        <v>294.07961924215846</v>
+      <c r="A285">
+        <v>294.07961924215851</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A286" s="1">
-        <v>1175.2574865837441</v>
+      <c r="A286">
+        <v>1175.2574865837439</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" s="1">
-        <v>194.39564368997893</v>
+      <c r="A287">
+        <v>194.3956436899789</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" s="1">
+      <c r="A288">
         <v>484.62499695018482</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A289" s="1">
+      <c r="A289">
         <v>81.820791783476238</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" s="1">
+      <c r="A290">
         <v>216.83048561323341</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" s="1">
-        <v>166.16341596586523</v>
+      <c r="A291">
+        <v>166.1634159658652</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" s="1">
-        <v>119.94525731901157</v>
+      <c r="A292">
+        <v>119.9452573190116</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" s="1">
-        <v>166.84843737976666</v>
+      <c r="A293">
+        <v>166.84843737976669</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" s="1">
+      <c r="A294">
         <v>776.85745898782318</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A295" s="1">
-        <v>268.29252853274653</v>
+      <c r="A295">
+        <v>268.29252853274647</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" s="1">
-        <v>100.90005371730453</v>
+      <c r="A296">
+        <v>100.9000537173045</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" s="1">
+      <c r="A297">
         <v>132.23708960717579</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A298" s="1">
+      <c r="A298">
         <v>355.01246274237479</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" s="1">
-        <v>287.47470278036786</v>
+      <c r="A299">
+        <v>287.47470278036792</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A300" s="1">
-        <v>218.61940586082983</v>
+      <c r="A300">
+        <v>218.6194058608298</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>